<commit_message>
Aggiunta analisi grafo topologico
</commit_message>
<xml_diff>
--- a/Documenti/Marco Catteneo/MRESim/logs/Analisi grafo topologico.xlsx
+++ b/Documenti/Marco Catteneo/MRESim/logs/Analisi grafo topologico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\Tesi\Documenti\Marco Catteneo\MRESim\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163DCD24-6148-479A-BEC7-38B32651F30D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B5809F-EC0C-4227-94CD-1F4743C0F968}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{1F295A6D-BD16-4A7A-B395-1E25C3F1794D}"/>
+    <workbookView xWindow="2295" yWindow="795" windowWidth="10245" windowHeight="11070" activeTab="1" xr2:uid="{1F295A6D-BD16-4A7A-B395-1E25C3F1794D}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -8647,8 +8647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{872A1278-AF11-4598-BBDF-3C7E9575775C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T38" sqref="T38"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Commit grosso dopo il passaggio a linux, ottimizzati metodi per fill delle matrici e gestione childMap in incrementalFW
</commit_message>
<xml_diff>
--- a/Documenti/Marco Catteneo/MRESim/logs/Analisi grafo topologico.xlsx
+++ b/Documenti/Marco Catteneo/MRESim/logs/Analisi grafo topologico.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\Tesi\Documenti\Marco Catteneo\MRESim\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B5809F-EC0C-4227-94CD-1F4743C0F968}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119AF526-B43E-4E7E-BECD-42C8C9E4F76D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="795" windowWidth="10245" windowHeight="11070" activeTab="1" xr2:uid="{1F295A6D-BD16-4A7A-B395-1E25C3F1794D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{1F295A6D-BD16-4A7A-B395-1E25C3F1794D}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
     <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Foglio1!$A$1:$H$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Foglio1!$A$1:$H$50</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -94,9 +94,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -195,11 +196,68 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="3"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
               <c:f>Foglio1!$K$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$L$2:$Q$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>113.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>115.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>150.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>119.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DCEF-49A9-BFBD-66F9CD3F7B36}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$K$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -246,12 +304,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$L$2:$Q$2</c:f>
+              <c:f>Foglio1!$L$3:$Q$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>99</c:v>
+                  <c:v>113.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>112</c:v>
@@ -260,7 +318,7 @@
                   <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>114</c:v>
+                  <c:v>118.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>114</c:v>
@@ -279,10 +337,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$K$3</c:f>
+              <c:f>Foglio1!$K$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -329,12 +387,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$L$3:$Q$3</c:f>
+              <c:f>Foglio1!$L$4:$Q$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>121.5</c:v>
+                  <c:v>123.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>125</c:v>
@@ -343,7 +401,7 @@
                   <c:v>113.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128.5</c:v>
+                  <c:v>123.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>124</c:v>
@@ -362,10 +420,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$K$4</c:f>
+              <c:f>Foglio1!$K$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -412,12 +470,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$L$4:$Q$4</c:f>
+              <c:f>Foglio1!$L$5:$Q$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>112</c:v>
+                  <c:v>115.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>116</c:v>
@@ -426,7 +484,7 @@
                   <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>111</c:v>
+                  <c:v>104.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>110</c:v>
@@ -727,11 +785,68 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="3"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$K$5</c:f>
+              <c:f>Foglio1!$K$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$L$6:$Q$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>133.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>134.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>137.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>152.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D597-4D07-B704-B00001AB0D3E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$K$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -778,12 +893,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$L$5:$Q$5</c:f>
+              <c:f>Foglio1!$L$7:$Q$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>155</c:v>
+                  <c:v>138.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>134.5</c:v>
@@ -792,7 +907,7 @@
                   <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>133.5</c:v>
+                  <c:v>136.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>140</c:v>
@@ -811,10 +926,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$K$6</c:f>
+              <c:f>Foglio1!$K$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -861,7 +976,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$L$6:$Q$6</c:f>
+              <c:f>Foglio1!$L$8:$Q$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -875,7 +990,7 @@
                   <c:v>141</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>134.5</c:v>
+                  <c:v>141.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>138.5</c:v>
@@ -894,10 +1009,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$K$7</c:f>
+              <c:f>Foglio1!$K$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -944,7 +1059,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$L$7:$Q$7</c:f>
+              <c:f>Foglio1!$L$9:$Q$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -958,7 +1073,7 @@
                   <c:v>141.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>143.5</c:v>
+                  <c:v>133.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>132.5</c:v>
@@ -1259,11 +1374,68 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="3"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$K$8</c:f>
+              <c:f>Foglio1!$K$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$L$10:$Q$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>85.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>89.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>101.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>105.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>113.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-12FC-4834-B6AD-AF734BFD57B6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$K$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1310,12 +1482,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$L$8:$Q$8</c:f>
+              <c:f>Foglio1!$L$11:$Q$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>84</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>81.5</c:v>
@@ -1324,7 +1496,7 @@
                   <c:v>86.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98</c:v>
+                  <c:v>81.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>85.5</c:v>
@@ -1343,10 +1515,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$K$9</c:f>
+              <c:f>Foglio1!$K$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1393,12 +1565,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$L$9:$Q$9</c:f>
+              <c:f>Foglio1!$L$12:$Q$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>76</c:v>
+                  <c:v>76.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>71.5</c:v>
@@ -1407,7 +1579,7 @@
                   <c:v>75.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>95.5</c:v>
+                  <c:v>86.3</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>93</c:v>
@@ -1426,10 +1598,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$K$10</c:f>
+              <c:f>Foglio1!$K$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1476,12 +1648,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$L$10:$Q$10</c:f>
+              <c:f>Foglio1!$L$13:$Q$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>70</c:v>
+                  <c:v>70.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>73.5</c:v>
@@ -1490,7 +1662,7 @@
                   <c:v>71.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80.5</c:v>
+                  <c:v>84.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>78.5</c:v>
@@ -1791,11 +1963,68 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="3"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$K$11</c:f>
+              <c:f>Foglio1!$K$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$L$14:$Q$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>57.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>63.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>79</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4076-4062-99B4-311DFD66B62D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$K$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1842,12 +2071,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$L$11:$Q$11</c:f>
+              <c:f>Foglio1!$L$15:$Q$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>56.5</c:v>
+                  <c:v>57.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>57.5</c:v>
@@ -1856,7 +2085,7 @@
                   <c:v>56.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>57</c:v>
+                  <c:v>59.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>57</c:v>
@@ -1875,10 +2104,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$K$12</c:f>
+              <c:f>Foglio1!$K$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1925,12 +2154,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$L$12:$Q$12</c:f>
+              <c:f>Foglio1!$L$16:$Q$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>55</c:v>
+                  <c:v>52.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>54</c:v>
@@ -1939,7 +2168,7 @@
                   <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56.5</c:v>
+                  <c:v>61.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>51</c:v>
@@ -1958,10 +2187,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$K$13</c:f>
+              <c:f>Foglio1!$K$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2008,12 +2237,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$L$13:$Q$13</c:f>
+              <c:f>Foglio1!$L$17:$Q$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>51.5</c:v>
+                  <c:v>51.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>55</c:v>
@@ -2022,7 +2251,7 @@
                   <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>62</c:v>
+                  <c:v>64.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>57</c:v>
@@ -2323,11 +2552,68 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="3"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$K$17</c:f>
+              <c:f>Foglio1!$K$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$L$22:$Q$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>73.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>87.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>91</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1F4C-4DCA-A7FB-7794F18CC5B3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$K$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2374,12 +2660,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$L$17:$Q$17</c:f>
+              <c:f>Foglio1!$L$23:$Q$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>70.5</c:v>
+                  <c:v>72.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>68</c:v>
@@ -2388,7 +2674,7 @@
                   <c:v>72.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>76</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>71</c:v>
@@ -2407,10 +2693,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$K$18</c:f>
+              <c:f>Foglio1!$K$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2457,12 +2743,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$L$18:$Q$18</c:f>
+              <c:f>Foglio1!$L$24:$Q$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>71.5</c:v>
+                  <c:v>72.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>69.5</c:v>
@@ -2471,7 +2757,7 @@
                   <c:v>71.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>78.5</c:v>
+                  <c:v>78.3</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>73.5</c:v>
@@ -2490,10 +2776,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$K$19</c:f>
+              <c:f>Foglio1!$K$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2540,12 +2826,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$L$19:$Q$19</c:f>
+              <c:f>Foglio1!$L$25:$Q$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>71</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>76.5</c:v>
@@ -2554,7 +2840,7 @@
                   <c:v>69.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>74</c:v>
+                  <c:v>74.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>74</c:v>
@@ -2855,11 +3141,68 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="3"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$K$14</c:f>
+              <c:f>Foglio1!$K$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$L$18:$Q$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>147.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>248.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>241.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>246.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4184-4B58-864E-3B1A706585F3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$K$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2906,12 +3249,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$L$14:$Q$14</c:f>
+              <c:f>Foglio1!$L$19:$Q$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>147.5</c:v>
+                  <c:v>149.30000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>142</c:v>
@@ -2920,7 +3263,7 @@
                   <c:v>141</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>155.5</c:v>
+                  <c:v>161.9</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>133.5</c:v>
@@ -2939,10 +3282,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$K$15</c:f>
+              <c:f>Foglio1!$K$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2989,12 +3332,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$L$15:$Q$15</c:f>
+              <c:f>Foglio1!$L$20:$Q$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>143</c:v>
+                  <c:v>134.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>144</c:v>
@@ -3003,7 +3346,7 @@
                   <c:v>134</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>181.5</c:v>
+                  <c:v>171.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>177.5</c:v>
@@ -3022,10 +3365,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$K$16</c:f>
+              <c:f>Foglio1!$K$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3072,7 +3415,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$L$16:$Q$16</c:f>
+              <c:f>Foglio1!$L$21:$Q$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -3086,7 +3429,7 @@
                   <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>134.5</c:v>
+                  <c:v>136.9</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>135.5</c:v>
@@ -7092,10 +7435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB94A998-842F-483C-AC6D-AE956C447F20}">
-  <dimension ref="A1:Q37"/>
+  <dimension ref="A1:Q49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7106,6 +7449,7 @@
     <col min="4" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7139,16 +7483,16 @@
       <c r="K1" t="s">
         <v>1</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="P1" t="s">
@@ -7163,55 +7507,53 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="D2">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="E2">
-        <v>126</v>
-      </c>
-      <c r="F2" s="1">
-        <v>107</v>
+        <v>105</v>
+      </c>
+      <c r="F2">
+        <v>101</v>
       </c>
       <c r="G2">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="H2">
-        <v>102</v>
+        <v>129</v>
       </c>
       <c r="J2">
         <v>1</v>
       </c>
       <c r="K2">
-        <v>9</v>
-      </c>
-      <c r="L2">
-        <f>AVERAGE(C2:C3)</f>
-        <v>99</v>
-      </c>
-      <c r="M2">
+        <v>8</v>
+      </c>
+      <c r="L2" s="2">
+        <v>113.4</v>
+      </c>
+      <c r="M2" s="2">
         <f t="shared" ref="M2:Q2" si="0">AVERAGE(D2:D3)</f>
-        <v>112</v>
-      </c>
-      <c r="N2">
+        <v>124</v>
+      </c>
+      <c r="N2" s="2">
         <f t="shared" si="0"/>
-        <v>126</v>
-      </c>
-      <c r="O2">
-        <f t="shared" si="0"/>
-        <v>114</v>
+        <v>115</v>
+      </c>
+      <c r="O2" s="2">
+        <v>115.9</v>
       </c>
       <c r="P2">
         <f t="shared" si="0"/>
-        <v>114</v>
+        <v>150.5</v>
       </c>
       <c r="Q2">
         <f t="shared" si="0"/>
-        <v>114</v>
+        <v>119.5</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -7219,55 +7561,53 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D3">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="E3">
-        <v>126</v>
-      </c>
-      <c r="F3" s="1">
-        <v>121</v>
+        <v>125</v>
+      </c>
+      <c r="F3">
+        <v>101</v>
       </c>
       <c r="G3">
-        <v>108</v>
+        <v>168</v>
       </c>
       <c r="H3">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
       <c r="K3">
-        <v>10</v>
-      </c>
-      <c r="L3">
-        <f>AVERAGE(C4:C5)</f>
-        <v>121.5</v>
-      </c>
-      <c r="M3">
+        <v>9</v>
+      </c>
+      <c r="L3" s="2">
+        <v>113.1</v>
+      </c>
+      <c r="M3" s="2">
         <f t="shared" ref="M3:Q3" si="1">AVERAGE(D4:D5)</f>
-        <v>125</v>
-      </c>
-      <c r="N3">
+        <v>112</v>
+      </c>
+      <c r="N3" s="2">
         <f t="shared" si="1"/>
-        <v>113.5</v>
-      </c>
-      <c r="O3">
-        <f t="shared" si="1"/>
-        <v>128.5</v>
+        <v>126</v>
+      </c>
+      <c r="O3" s="2">
+        <v>118.1</v>
       </c>
       <c r="P3">
         <f t="shared" si="1"/>
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="Q3">
         <f t="shared" si="1"/>
-        <v>132.5</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -7275,55 +7615,53 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="D4">
+        <v>111</v>
+      </c>
+      <c r="E4">
         <v>126</v>
       </c>
-      <c r="E4">
-        <v>113</v>
-      </c>
-      <c r="F4">
-        <v>137</v>
+      <c r="F4" s="1">
+        <v>107</v>
       </c>
       <c r="G4">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H4">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="J4">
         <v>1</v>
       </c>
       <c r="K4">
-        <v>11</v>
-      </c>
-      <c r="L4">
-        <f>AVERAGE(C6:C7)</f>
-        <v>112</v>
-      </c>
-      <c r="M4">
+        <v>10</v>
+      </c>
+      <c r="L4" s="2">
+        <v>123.4</v>
+      </c>
+      <c r="M4" s="2">
         <f t="shared" ref="M4:Q4" si="2">AVERAGE(D6:D7)</f>
-        <v>116</v>
-      </c>
-      <c r="N4">
+        <v>125</v>
+      </c>
+      <c r="N4" s="2">
         <f t="shared" si="2"/>
-        <v>106</v>
-      </c>
-      <c r="O4">
-        <f t="shared" si="2"/>
-        <v>111</v>
+        <v>113.5</v>
+      </c>
+      <c r="O4" s="2">
+        <v>123.7</v>
       </c>
       <c r="P4">
         <f t="shared" si="2"/>
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="Q4">
         <f t="shared" si="2"/>
-        <v>101.5</v>
+        <v>132.5</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -7331,55 +7669,53 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="D5">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="E5">
-        <v>114</v>
-      </c>
-      <c r="F5">
-        <v>120</v>
+        <v>126</v>
+      </c>
+      <c r="F5" s="1">
+        <v>121</v>
       </c>
       <c r="G5">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="H5">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="J5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K5">
-        <v>9</v>
-      </c>
-      <c r="L5">
-        <f>AVERAGE(C8:C9)</f>
-        <v>155</v>
-      </c>
-      <c r="M5">
+        <v>11</v>
+      </c>
+      <c r="L5" s="2">
+        <v>115.9</v>
+      </c>
+      <c r="M5" s="2">
         <f t="shared" ref="M5:Q5" si="3">AVERAGE(D8:D9)</f>
-        <v>134.5</v>
-      </c>
-      <c r="N5">
+        <v>116</v>
+      </c>
+      <c r="N5" s="2">
         <f t="shared" si="3"/>
-        <v>131</v>
-      </c>
-      <c r="O5">
-        <f t="shared" si="3"/>
-        <v>133.5</v>
+        <v>106</v>
+      </c>
+      <c r="O5" s="2">
+        <v>104.5</v>
       </c>
       <c r="P5">
         <f t="shared" si="3"/>
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="Q5">
         <f t="shared" si="3"/>
-        <v>137</v>
+        <v>101.5</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -7387,55 +7723,53 @@
         <v>1</v>
       </c>
       <c r="B6">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="D6">
+        <v>126</v>
+      </c>
+      <c r="E6">
+        <v>113</v>
+      </c>
+      <c r="F6">
+        <v>137</v>
+      </c>
+      <c r="G6">
         <v>119</v>
       </c>
-      <c r="E6">
-        <v>105</v>
-      </c>
-      <c r="F6">
-        <v>109</v>
-      </c>
-      <c r="G6">
-        <v>115</v>
-      </c>
       <c r="H6">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="J6">
         <v>2</v>
       </c>
       <c r="K6">
-        <v>10</v>
-      </c>
-      <c r="L6">
-        <f>AVERAGE(C10:C11)</f>
-        <v>174</v>
-      </c>
-      <c r="M6">
+        <v>8</v>
+      </c>
+      <c r="L6" s="2">
+        <v>133.9</v>
+      </c>
+      <c r="M6" s="2">
         <f t="shared" ref="M6:Q6" si="4">AVERAGE(D10:D11)</f>
-        <v>141</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="4"/>
-        <v>141</v>
-      </c>
-      <c r="O6">
+        <v>134</v>
+      </c>
+      <c r="N6" s="2">
         <f t="shared" si="4"/>
         <v>134.5</v>
       </c>
+      <c r="O6" s="2">
+        <v>137.69999999999999</v>
+      </c>
       <c r="P6">
         <f t="shared" si="4"/>
-        <v>138.5</v>
+        <v>140</v>
       </c>
       <c r="Q6">
         <f t="shared" si="4"/>
-        <v>142</v>
+        <v>152.5</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -7443,167 +7777,161 @@
         <v>1</v>
       </c>
       <c r="B7">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="D7">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="E7">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="F7">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="G7">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="H7">
-        <v>110</v>
+        <v>133</v>
       </c>
       <c r="J7">
         <v>2</v>
       </c>
       <c r="K7">
-        <v>11</v>
-      </c>
-      <c r="L7">
-        <f>AVERAGE(C12:C13)</f>
-        <v>146</v>
-      </c>
-      <c r="M7">
+        <v>9</v>
+      </c>
+      <c r="L7" s="2">
+        <v>138.4</v>
+      </c>
+      <c r="M7" s="2">
         <f t="shared" ref="M7:Q7" si="5">AVERAGE(D12:D13)</f>
-        <v>137.5</v>
-      </c>
-      <c r="N7">
+        <v>134.5</v>
+      </c>
+      <c r="N7" s="2">
         <f t="shared" si="5"/>
-        <v>141.5</v>
-      </c>
-      <c r="O7">
-        <f t="shared" si="5"/>
-        <v>143.5</v>
+        <v>131</v>
+      </c>
+      <c r="O7" s="2">
+        <v>136.5</v>
       </c>
       <c r="P7">
         <f t="shared" si="5"/>
-        <v>132.5</v>
+        <v>140</v>
       </c>
       <c r="Q7">
         <f t="shared" si="5"/>
-        <v>131.5</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>111</v>
+      </c>
+      <c r="D8">
+        <v>119</v>
+      </c>
+      <c r="E8">
+        <v>105</v>
+      </c>
+      <c r="F8">
+        <v>109</v>
+      </c>
+      <c r="G8">
+        <v>115</v>
+      </c>
+      <c r="H8">
+        <v>93</v>
+      </c>
+      <c r="J8">
         <v>2</v>
       </c>
-      <c r="B8">
-        <v>9</v>
-      </c>
-      <c r="C8">
-        <v>159</v>
-      </c>
-      <c r="D8">
-        <v>133</v>
-      </c>
-      <c r="E8">
-        <v>131</v>
-      </c>
-      <c r="F8" s="1">
-        <v>133</v>
-      </c>
-      <c r="G8">
-        <v>139</v>
-      </c>
-      <c r="H8">
-        <v>132</v>
-      </c>
-      <c r="J8">
-        <v>3</v>
-      </c>
       <c r="K8">
-        <v>9</v>
-      </c>
-      <c r="L8">
-        <f>AVERAGE(C14:C15)</f>
-        <v>84</v>
-      </c>
-      <c r="M8">
+        <v>10</v>
+      </c>
+      <c r="L8" s="2">
+        <v>174</v>
+      </c>
+      <c r="M8" s="2">
         <f t="shared" ref="M8:Q8" si="6">AVERAGE(D14:D15)</f>
-        <v>81.5</v>
-      </c>
-      <c r="N8">
+        <v>141</v>
+      </c>
+      <c r="N8" s="2">
         <f t="shared" si="6"/>
-        <v>86.5</v>
-      </c>
-      <c r="O8">
-        <f t="shared" si="6"/>
-        <v>98</v>
+        <v>141</v>
+      </c>
+      <c r="O8" s="2">
+        <v>141.1</v>
       </c>
       <c r="P8">
         <f t="shared" si="6"/>
-        <v>85.5</v>
+        <v>138.5</v>
       </c>
       <c r="Q8">
         <f t="shared" si="6"/>
-        <v>90.5</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>113</v>
+      </c>
+      <c r="D9">
+        <v>113</v>
+      </c>
+      <c r="E9">
+        <v>107</v>
+      </c>
+      <c r="F9">
+        <v>113</v>
+      </c>
+      <c r="G9">
+        <v>105</v>
+      </c>
+      <c r="H9">
+        <v>110</v>
+      </c>
+      <c r="J9">
         <v>2</v>
       </c>
-      <c r="B9">
-        <v>9</v>
-      </c>
-      <c r="C9">
-        <v>151</v>
-      </c>
-      <c r="D9">
-        <v>136</v>
-      </c>
-      <c r="E9">
-        <v>131</v>
-      </c>
-      <c r="F9" s="1">
-        <v>134</v>
-      </c>
-      <c r="G9">
-        <v>141</v>
-      </c>
-      <c r="H9">
-        <v>142</v>
-      </c>
-      <c r="J9">
-        <v>3</v>
-      </c>
       <c r="K9">
-        <v>10</v>
-      </c>
-      <c r="L9">
-        <f>AVERAGE(C16:C17)</f>
-        <v>76</v>
-      </c>
-      <c r="M9">
+        <v>11</v>
+      </c>
+      <c r="L9" s="2">
+        <v>146</v>
+      </c>
+      <c r="M9" s="2">
         <f t="shared" ref="M9:Q9" si="7">AVERAGE(D16:D17)</f>
-        <v>71.5</v>
-      </c>
-      <c r="N9">
+        <v>137.5</v>
+      </c>
+      <c r="N9" s="2">
         <f t="shared" si="7"/>
-        <v>75.5</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="7"/>
-        <v>95.5</v>
+        <v>141.5</v>
+      </c>
+      <c r="O9" s="2">
+        <v>133.6</v>
       </c>
       <c r="P9">
         <f t="shared" si="7"/>
-        <v>93</v>
+        <v>132.5</v>
       </c>
       <c r="Q9">
         <f t="shared" si="7"/>
-        <v>86.5</v>
+        <v>131.5</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -7611,55 +7939,53 @@
         <v>2</v>
       </c>
       <c r="B10">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10">
-        <v>174</v>
+        <v>132</v>
       </c>
       <c r="D10">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="E10">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="F10">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G10">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H10">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="J10">
         <v>3</v>
       </c>
       <c r="K10">
-        <v>11</v>
-      </c>
-      <c r="L10">
-        <f>AVERAGE(C18:C19)</f>
-        <v>70</v>
-      </c>
-      <c r="M10">
-        <f t="shared" ref="M10:Q10" si="8">AVERAGE(D18:D19)</f>
-        <v>73.5</v>
-      </c>
-      <c r="N10">
+        <v>8</v>
+      </c>
+      <c r="L10" s="2">
+        <v>85.4</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" ref="M10:P10" si="8">AVERAGE(D18:D19)</f>
+        <v>92</v>
+      </c>
+      <c r="N10" s="2">
         <f t="shared" si="8"/>
-        <v>71.5</v>
-      </c>
-      <c r="O10">
-        <f t="shared" si="8"/>
-        <v>80.5</v>
+        <v>89.5</v>
+      </c>
+      <c r="O10" s="2">
+        <v>101.6</v>
       </c>
       <c r="P10">
         <f t="shared" si="8"/>
-        <v>78.5</v>
+        <v>105.5</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="8"/>
-        <v>83</v>
+        <f>AVERAGE(H18:H19)</f>
+        <v>113.5</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -7667,55 +7993,53 @@
         <v>2</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C11">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="D11">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="E11">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="F11">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="G11">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H11">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="J11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K11">
         <v>9</v>
       </c>
-      <c r="L11">
-        <f>AVERAGE(C20:C21)</f>
-        <v>56.5</v>
-      </c>
-      <c r="M11">
+      <c r="L11" s="2">
+        <v>83</v>
+      </c>
+      <c r="M11" s="2">
         <f t="shared" ref="M11:Q11" si="9">AVERAGE(D20:D21)</f>
-        <v>57.5</v>
-      </c>
-      <c r="N11">
+        <v>81.5</v>
+      </c>
+      <c r="N11" s="2">
         <f t="shared" si="9"/>
-        <v>56.5</v>
-      </c>
-      <c r="O11">
-        <f t="shared" si="9"/>
-        <v>57</v>
+        <v>86.5</v>
+      </c>
+      <c r="O11" s="2">
+        <v>81.2</v>
       </c>
       <c r="P11">
         <f t="shared" si="9"/>
-        <v>57</v>
+        <v>85.5</v>
       </c>
       <c r="Q11">
         <f t="shared" si="9"/>
-        <v>57</v>
+        <v>90.5</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -7723,55 +8047,53 @@
         <v>2</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="D12">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E12">
-        <v>142</v>
-      </c>
-      <c r="F12">
-        <v>155</v>
+        <v>131</v>
+      </c>
+      <c r="F12" s="1">
+        <v>133</v>
       </c>
       <c r="G12">
+        <v>139</v>
+      </c>
+      <c r="H12">
         <v>132</v>
       </c>
-      <c r="H12">
-        <v>130</v>
-      </c>
       <c r="J12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K12">
         <v>10</v>
       </c>
-      <c r="L12">
-        <f>AVERAGE(C22:C23)</f>
-        <v>55</v>
-      </c>
-      <c r="M12">
+      <c r="L12" s="2">
+        <v>76.599999999999994</v>
+      </c>
+      <c r="M12" s="2">
         <f t="shared" ref="M12:Q12" si="10">AVERAGE(D22:D23)</f>
-        <v>54</v>
-      </c>
-      <c r="N12">
+        <v>71.5</v>
+      </c>
+      <c r="N12" s="2">
         <f t="shared" si="10"/>
-        <v>46</v>
-      </c>
-      <c r="O12">
-        <f t="shared" si="10"/>
-        <v>56.5</v>
+        <v>75.5</v>
+      </c>
+      <c r="O12" s="2">
+        <v>86.3</v>
       </c>
       <c r="P12">
         <f t="shared" si="10"/>
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="Q12">
         <f t="shared" si="10"/>
-        <v>51</v>
+        <v>86.5</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -7779,279 +8101,269 @@
         <v>2</v>
       </c>
       <c r="B13">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C13">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="D13">
+        <v>136</v>
+      </c>
+      <c r="E13">
+        <v>131</v>
+      </c>
+      <c r="F13" s="1">
         <v>134</v>
       </c>
-      <c r="E13">
+      <c r="G13">
         <v>141</v>
       </c>
-      <c r="F13">
-        <v>132</v>
-      </c>
-      <c r="G13">
-        <v>133</v>
-      </c>
       <c r="H13">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="J13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K13">
         <v>11</v>
       </c>
-      <c r="L13">
-        <f>AVERAGE(C24:C25)</f>
-        <v>51.5</v>
-      </c>
-      <c r="M13">
+      <c r="L13" s="2">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="M13" s="2">
         <f t="shared" ref="M13:Q13" si="11">AVERAGE(D24:D25)</f>
-        <v>55</v>
-      </c>
-      <c r="N13">
+        <v>73.5</v>
+      </c>
+      <c r="N13" s="2">
         <f t="shared" si="11"/>
-        <v>44</v>
-      </c>
-      <c r="O13">
-        <f t="shared" si="11"/>
-        <v>62</v>
+        <v>71.5</v>
+      </c>
+      <c r="O13" s="2">
+        <v>84.7</v>
       </c>
       <c r="P13">
         <f t="shared" si="11"/>
-        <v>57</v>
+        <v>78.5</v>
       </c>
       <c r="Q13">
         <f t="shared" si="11"/>
-        <v>44</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B14">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C14">
-        <v>84</v>
+        <v>174</v>
       </c>
       <c r="D14">
-        <v>82</v>
+        <v>141</v>
       </c>
       <c r="E14">
-        <v>89</v>
+        <v>141</v>
       </c>
       <c r="F14">
-        <v>96</v>
+        <v>140</v>
       </c>
       <c r="G14">
-        <v>101</v>
+        <v>136</v>
       </c>
       <c r="H14">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="J14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K14">
-        <v>9</v>
-      </c>
-      <c r="L14">
-        <f>AVERAGE(C26:C27)</f>
-        <v>147.5</v>
-      </c>
-      <c r="M14">
+        <v>8</v>
+      </c>
+      <c r="L14" s="2">
+        <v>57.2</v>
+      </c>
+      <c r="M14" s="2">
         <f t="shared" ref="M14:Q14" si="12">AVERAGE(D26:D27)</f>
-        <v>142</v>
-      </c>
-      <c r="N14">
+        <v>58</v>
+      </c>
+      <c r="N14" s="2">
         <f t="shared" si="12"/>
-        <v>141</v>
-      </c>
-      <c r="O14">
-        <f t="shared" si="12"/>
-        <v>155.5</v>
+        <v>58</v>
+      </c>
+      <c r="O14" s="2">
+        <v>63.8</v>
       </c>
       <c r="P14">
         <f t="shared" si="12"/>
-        <v>133.5</v>
+        <v>79</v>
       </c>
       <c r="Q14">
         <f t="shared" si="12"/>
-        <v>142.5</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>174</v>
+      </c>
+      <c r="D15">
+        <v>141</v>
+      </c>
+      <c r="E15">
+        <v>141</v>
+      </c>
+      <c r="F15">
+        <v>129</v>
+      </c>
+      <c r="G15">
+        <v>141</v>
+      </c>
+      <c r="H15">
+        <v>147</v>
+      </c>
+      <c r="J15">
+        <v>4</v>
+      </c>
+      <c r="K15">
         <v>9</v>
       </c>
-      <c r="C15">
-        <v>84</v>
-      </c>
-      <c r="D15">
-        <v>81</v>
-      </c>
-      <c r="E15">
-        <v>84</v>
-      </c>
-      <c r="F15">
-        <v>100</v>
-      </c>
-      <c r="G15">
-        <v>70</v>
-      </c>
-      <c r="H15">
-        <v>84</v>
-      </c>
-      <c r="J15">
-        <v>5</v>
-      </c>
-      <c r="K15">
-        <v>10</v>
-      </c>
-      <c r="L15">
-        <f>AVERAGE(C28:C29)</f>
-        <v>143</v>
-      </c>
-      <c r="M15">
+      <c r="L15" s="2">
+        <v>57.4</v>
+      </c>
+      <c r="M15" s="2">
         <f t="shared" ref="M15:Q15" si="13">AVERAGE(D28:D29)</f>
-        <v>144</v>
-      </c>
-      <c r="N15">
+        <v>57.5</v>
+      </c>
+      <c r="N15" s="2">
         <f t="shared" si="13"/>
-        <v>134</v>
-      </c>
-      <c r="O15">
-        <f t="shared" si="13"/>
-        <v>181.5</v>
+        <v>56.5</v>
+      </c>
+      <c r="O15" s="2">
+        <v>59.2</v>
       </c>
       <c r="P15">
         <f t="shared" si="13"/>
-        <v>177.5</v>
+        <v>57</v>
       </c>
       <c r="Q15">
         <f t="shared" si="13"/>
-        <v>240</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B16">
+        <v>11</v>
+      </c>
+      <c r="C16">
+        <v>146</v>
+      </c>
+      <c r="D16">
+        <v>141</v>
+      </c>
+      <c r="E16">
+        <v>142</v>
+      </c>
+      <c r="F16">
+        <v>155</v>
+      </c>
+      <c r="G16">
+        <v>132</v>
+      </c>
+      <c r="H16">
+        <v>130</v>
+      </c>
+      <c r="J16">
+        <v>4</v>
+      </c>
+      <c r="K16">
         <v>10</v>
       </c>
-      <c r="C16">
-        <v>72</v>
-      </c>
-      <c r="D16">
-        <v>69</v>
-      </c>
-      <c r="E16">
-        <v>74</v>
-      </c>
-      <c r="F16">
-        <v>106</v>
-      </c>
-      <c r="G16">
-        <v>92</v>
-      </c>
-      <c r="H16">
-        <v>85</v>
-      </c>
-      <c r="J16">
-        <v>5</v>
-      </c>
-      <c r="K16">
-        <v>11</v>
-      </c>
-      <c r="L16">
-        <f>AVERAGE(C30:C31)</f>
-        <v>137</v>
-      </c>
-      <c r="M16">
+      <c r="L16" s="2">
+        <v>52.6</v>
+      </c>
+      <c r="M16" s="2">
         <f t="shared" ref="M16:Q16" si="14">AVERAGE(D30:D31)</f>
-        <v>123</v>
-      </c>
-      <c r="N16">
+        <v>54</v>
+      </c>
+      <c r="N16" s="2">
         <f t="shared" si="14"/>
-        <v>133</v>
-      </c>
-      <c r="O16">
-        <f t="shared" si="14"/>
-        <v>134.5</v>
+        <v>46</v>
+      </c>
+      <c r="O16" s="2">
+        <v>61.4</v>
       </c>
       <c r="P16">
         <f t="shared" si="14"/>
-        <v>135.5</v>
+        <v>51</v>
       </c>
       <c r="Q16">
         <f t="shared" si="14"/>
-        <v>156</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B17">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C17">
-        <v>80</v>
+        <v>146</v>
       </c>
       <c r="D17">
-        <v>74</v>
+        <v>134</v>
       </c>
       <c r="E17">
-        <v>77</v>
+        <v>141</v>
       </c>
       <c r="F17">
-        <v>85</v>
+        <v>132</v>
       </c>
       <c r="G17">
-        <v>94</v>
+        <v>133</v>
       </c>
       <c r="H17">
-        <v>88</v>
+        <v>133</v>
       </c>
       <c r="J17">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K17">
-        <v>9</v>
-      </c>
-      <c r="L17">
-        <f>AVERAGE(C32:C33)</f>
-        <v>70.5</v>
-      </c>
-      <c r="M17">
+        <v>11</v>
+      </c>
+      <c r="L17" s="2">
+        <v>51.6</v>
+      </c>
+      <c r="M17" s="2">
         <f t="shared" ref="M17:Q17" si="15">AVERAGE(D32:D33)</f>
-        <v>68</v>
-      </c>
-      <c r="N17">
+        <v>55</v>
+      </c>
+      <c r="N17" s="2">
         <f t="shared" si="15"/>
-        <v>72.5</v>
-      </c>
-      <c r="O17">
-        <f t="shared" si="15"/>
-        <v>76</v>
+        <v>44</v>
+      </c>
+      <c r="O17" s="2">
+        <v>64.8</v>
       </c>
       <c r="P17">
         <f t="shared" si="15"/>
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="Q17">
         <f t="shared" si="15"/>
-        <v>73.5</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -8059,55 +8371,53 @@
         <v>3</v>
       </c>
       <c r="B18">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C18">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="D18">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="E18">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="F18">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="G18">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="H18">
-        <v>88</v>
+        <v>126</v>
       </c>
       <c r="J18">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K18">
-        <v>10</v>
-      </c>
-      <c r="L18">
-        <f>AVERAGE(C34:C35)</f>
-        <v>71.5</v>
-      </c>
-      <c r="M18">
+        <v>8</v>
+      </c>
+      <c r="L18" s="2">
+        <v>147.69999999999999</v>
+      </c>
+      <c r="M18" s="2">
         <f t="shared" ref="M18:Q18" si="16">AVERAGE(D34:D35)</f>
-        <v>69.5</v>
-      </c>
-      <c r="N18">
+        <v>133</v>
+      </c>
+      <c r="N18" s="2">
         <f t="shared" si="16"/>
-        <v>71.5</v>
-      </c>
-      <c r="O18">
-        <f t="shared" si="16"/>
-        <v>78.5</v>
+        <v>129</v>
+      </c>
+      <c r="O18" s="2">
+        <v>248.9</v>
       </c>
       <c r="P18">
         <f t="shared" si="16"/>
-        <v>73.5</v>
+        <v>241.5</v>
       </c>
       <c r="Q18">
         <f t="shared" si="16"/>
-        <v>77.5</v>
+        <v>246.5</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -8115,528 +8425,1006 @@
         <v>3</v>
       </c>
       <c r="B19">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C19">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="D19">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="E19">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="F19">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="G19">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="H19">
-        <v>78</v>
+        <v>101</v>
       </c>
       <c r="J19">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K19">
-        <v>11</v>
-      </c>
-      <c r="L19">
-        <f>AVERAGE(C36:C37)</f>
-        <v>71</v>
-      </c>
-      <c r="M19">
+        <v>9</v>
+      </c>
+      <c r="L19" s="2">
+        <v>149.30000000000001</v>
+      </c>
+      <c r="M19" s="2">
         <f t="shared" ref="M19:Q19" si="17">AVERAGE(D36:D37)</f>
-        <v>76.5</v>
-      </c>
-      <c r="N19">
+        <v>142</v>
+      </c>
+      <c r="N19" s="2">
         <f t="shared" si="17"/>
-        <v>69.5</v>
-      </c>
-      <c r="O19">
-        <f t="shared" si="17"/>
-        <v>74</v>
+        <v>141</v>
+      </c>
+      <c r="O19" s="2">
+        <v>161.9</v>
       </c>
       <c r="P19">
         <f t="shared" si="17"/>
-        <v>74</v>
+        <v>133.5</v>
       </c>
       <c r="Q19">
         <f t="shared" si="17"/>
-        <v>75.5</v>
+        <v>142.5</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20">
         <v>9</v>
       </c>
       <c r="C20">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="D20">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="E20">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="F20">
-        <v>57</v>
+        <v>96</v>
       </c>
       <c r="G20">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="H20">
-        <v>57</v>
+        <v>97</v>
+      </c>
+      <c r="J20">
+        <v>5</v>
+      </c>
+      <c r="K20">
+        <v>10</v>
+      </c>
+      <c r="L20" s="2">
+        <v>134.1</v>
+      </c>
+      <c r="M20" s="2">
+        <f t="shared" ref="M20:Q20" si="18">AVERAGE(D38:D39)</f>
+        <v>144</v>
+      </c>
+      <c r="N20" s="2">
+        <f t="shared" si="18"/>
+        <v>134</v>
+      </c>
+      <c r="O20" s="2">
+        <v>171.1</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="18"/>
+        <v>177.5</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="18"/>
+        <v>240</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B21">
         <v>9</v>
       </c>
       <c r="C21">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="D21">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="E21">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="F21">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="G21">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="H21">
-        <v>57</v>
+        <v>84</v>
+      </c>
+      <c r="J21">
+        <v>5</v>
+      </c>
+      <c r="K21">
+        <v>11</v>
+      </c>
+      <c r="L21" s="2">
+        <v>137</v>
+      </c>
+      <c r="M21" s="2">
+        <f t="shared" ref="M21:Q21" si="19">AVERAGE(D40:D41)</f>
+        <v>123</v>
+      </c>
+      <c r="N21" s="2">
+        <f t="shared" si="19"/>
+        <v>133</v>
+      </c>
+      <c r="O21" s="2">
+        <v>136.9</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="19"/>
+        <v>135.5</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="19"/>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B22">
         <v>10</v>
       </c>
       <c r="C22">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D22">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="E22">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="F22">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="G22">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="H22">
-        <v>51</v>
+        <v>85</v>
+      </c>
+      <c r="J22">
+        <v>6</v>
+      </c>
+      <c r="K22">
+        <v>8</v>
+      </c>
+      <c r="L22" s="2">
+        <v>73.2</v>
+      </c>
+      <c r="M22" s="2">
+        <f t="shared" ref="M22:Q22" si="20">AVERAGE(D42:D43)</f>
+        <v>71</v>
+      </c>
+      <c r="N22" s="2">
+        <f t="shared" si="20"/>
+        <v>76</v>
+      </c>
+      <c r="O22" s="2">
+        <v>87.8</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="20"/>
+        <v>88</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="20"/>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B23">
         <v>10</v>
       </c>
       <c r="C23">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="D23">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="E23">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F23">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="G23">
-        <v>51</v>
+        <v>94</v>
       </c>
       <c r="H23">
-        <v>51</v>
+        <v>88</v>
+      </c>
+      <c r="J23">
+        <v>6</v>
+      </c>
+      <c r="K23">
+        <v>9</v>
+      </c>
+      <c r="L23" s="2">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="M23" s="2">
+        <f t="shared" ref="M23:Q23" si="21">AVERAGE(D44:D45)</f>
+        <v>68</v>
+      </c>
+      <c r="N23" s="2">
+        <f t="shared" si="21"/>
+        <v>72.5</v>
+      </c>
+      <c r="O23" s="2">
+        <v>74</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="21"/>
+        <v>71</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="21"/>
+        <v>73.5</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B24">
         <v>11</v>
       </c>
       <c r="C24">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="D24">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="E24">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="F24">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="G24">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="H24">
-        <v>44</v>
+        <v>88</v>
+      </c>
+      <c r="J24">
+        <v>6</v>
+      </c>
+      <c r="K24">
+        <v>10</v>
+      </c>
+      <c r="L24" s="2">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="M24" s="2">
+        <f t="shared" ref="M24:Q24" si="22">AVERAGE(D46:D47)</f>
+        <v>69.5</v>
+      </c>
+      <c r="N24" s="2">
+        <f t="shared" si="22"/>
+        <v>71.5</v>
+      </c>
+      <c r="O24" s="2">
+        <v>78.3</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="22"/>
+        <v>73.5</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="22"/>
+        <v>77.5</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B25">
         <v>11</v>
       </c>
       <c r="C25">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="D25">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="E25">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="F25">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="G25">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="H25">
-        <v>44</v>
+        <v>78</v>
+      </c>
+      <c r="J25">
+        <v>6</v>
+      </c>
+      <c r="K25">
+        <v>11</v>
+      </c>
+      <c r="L25" s="2">
+        <v>73</v>
+      </c>
+      <c r="M25" s="2">
+        <f t="shared" ref="M25:Q25" si="23">AVERAGE(D48:D49)</f>
+        <v>76.5</v>
+      </c>
+      <c r="N25" s="2">
+        <f t="shared" si="23"/>
+        <v>69.5</v>
+      </c>
+      <c r="O25" s="2">
+        <v>74.7</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="23"/>
+        <v>74</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="23"/>
+        <v>75.5</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B26">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C26">
-        <v>155</v>
+        <v>57</v>
       </c>
       <c r="D26">
-        <v>141</v>
+        <v>58</v>
       </c>
       <c r="E26">
-        <v>141</v>
+        <v>58</v>
       </c>
       <c r="F26">
-        <v>157</v>
+        <v>62</v>
       </c>
       <c r="G26">
-        <v>134</v>
+        <v>79</v>
       </c>
       <c r="H26">
-        <v>131</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B27">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27">
-        <v>140</v>
+        <v>58</v>
       </c>
       <c r="D27">
-        <v>143</v>
+        <v>58</v>
       </c>
       <c r="E27">
-        <v>141</v>
+        <v>58</v>
       </c>
       <c r="F27">
-        <v>154</v>
+        <v>60</v>
       </c>
       <c r="G27">
-        <v>133</v>
+        <v>79</v>
       </c>
       <c r="H27">
-        <v>154</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B28">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C28">
-        <v>128</v>
+        <v>57</v>
       </c>
       <c r="D28">
-        <v>156</v>
+        <v>57</v>
       </c>
       <c r="E28">
-        <v>129</v>
+        <v>58</v>
       </c>
       <c r="F28">
-        <v>185</v>
+        <v>57</v>
       </c>
       <c r="G28">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="H28">
-        <v>265</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B29">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C29">
-        <v>158</v>
+        <v>56</v>
       </c>
       <c r="D29">
-        <v>132</v>
+        <v>58</v>
       </c>
       <c r="E29">
-        <v>139</v>
+        <v>55</v>
       </c>
       <c r="F29">
-        <v>178</v>
+        <v>57</v>
       </c>
       <c r="G29">
-        <v>182</v>
+        <v>57</v>
       </c>
       <c r="H29">
-        <v>215</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B30">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C30">
-        <v>131</v>
+        <v>59</v>
       </c>
       <c r="D30">
-        <v>128</v>
+        <v>54</v>
       </c>
       <c r="E30">
-        <v>128</v>
+        <v>46</v>
       </c>
       <c r="F30">
-        <v>136</v>
+        <v>62</v>
       </c>
       <c r="G30">
-        <v>135</v>
+        <v>51</v>
       </c>
       <c r="H30">
-        <v>154</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B31">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C31">
-        <v>143</v>
+        <v>51</v>
       </c>
       <c r="D31">
-        <v>118</v>
+        <v>54</v>
       </c>
       <c r="E31">
-        <v>138</v>
+        <v>46</v>
       </c>
       <c r="F31">
-        <v>133</v>
+        <v>51</v>
       </c>
       <c r="G31">
-        <v>136</v>
+        <v>51</v>
       </c>
       <c r="H31">
-        <v>158</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B32">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C32">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="D32">
+        <v>55</v>
+      </c>
+      <c r="E32">
+        <v>44</v>
+      </c>
+      <c r="F32">
         <v>68</v>
       </c>
-      <c r="E32">
-        <v>72</v>
-      </c>
-      <c r="F32">
-        <v>77</v>
-      </c>
       <c r="G32">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="H32">
-        <v>77</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B33">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C33">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D33">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="E33">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="F33">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="G33">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="H33">
-        <v>70</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B34">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C34">
-        <v>72</v>
+        <v>154</v>
       </c>
       <c r="D34">
-        <v>70</v>
+        <v>133</v>
       </c>
       <c r="E34">
-        <v>74</v>
+        <v>129</v>
       </c>
       <c r="F34">
-        <v>79</v>
+        <v>169</v>
       </c>
       <c r="G34">
-        <v>76</v>
+        <v>190</v>
       </c>
       <c r="H34">
-        <v>77</v>
+        <v>231</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B35">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C35">
-        <v>71</v>
+        <v>136</v>
       </c>
       <c r="D35">
-        <v>69</v>
+        <v>133</v>
       </c>
       <c r="E35">
-        <v>69</v>
+        <v>129</v>
       </c>
       <c r="F35">
-        <v>78</v>
+        <v>189</v>
       </c>
       <c r="G35">
-        <v>71</v>
+        <v>293</v>
       </c>
       <c r="H35">
-        <v>78</v>
+        <v>262</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B36">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C36">
-        <v>72</v>
+        <v>155</v>
       </c>
       <c r="D36">
-        <v>76</v>
+        <v>141</v>
       </c>
       <c r="E36">
-        <v>69</v>
+        <v>141</v>
       </c>
       <c r="F36">
-        <v>74</v>
+        <v>157</v>
       </c>
       <c r="G36">
-        <v>75</v>
+        <v>134</v>
       </c>
       <c r="H36">
-        <v>72</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <v>9</v>
+      </c>
+      <c r="C37">
+        <v>140</v>
+      </c>
+      <c r="D37">
+        <v>143</v>
+      </c>
+      <c r="E37">
+        <v>141</v>
+      </c>
+      <c r="F37">
+        <v>154</v>
+      </c>
+      <c r="G37">
+        <v>133</v>
+      </c>
+      <c r="H37">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>5</v>
+      </c>
+      <c r="B38">
+        <v>10</v>
+      </c>
+      <c r="C38">
+        <v>128</v>
+      </c>
+      <c r="D38">
+        <v>156</v>
+      </c>
+      <c r="E38">
+        <v>129</v>
+      </c>
+      <c r="F38">
+        <v>185</v>
+      </c>
+      <c r="G38">
+        <v>173</v>
+      </c>
+      <c r="H38">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>5</v>
+      </c>
+      <c r="B39">
+        <v>10</v>
+      </c>
+      <c r="C39">
+        <v>158</v>
+      </c>
+      <c r="D39">
+        <v>132</v>
+      </c>
+      <c r="E39">
+        <v>139</v>
+      </c>
+      <c r="F39">
+        <v>178</v>
+      </c>
+      <c r="G39">
+        <v>182</v>
+      </c>
+      <c r="H39">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>5</v>
+      </c>
+      <c r="B40">
+        <v>11</v>
+      </c>
+      <c r="C40">
+        <v>131</v>
+      </c>
+      <c r="D40">
+        <v>128</v>
+      </c>
+      <c r="E40">
+        <v>128</v>
+      </c>
+      <c r="F40">
+        <v>136</v>
+      </c>
+      <c r="G40">
+        <v>135</v>
+      </c>
+      <c r="H40">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>11</v>
+      </c>
+      <c r="C41">
+        <v>143</v>
+      </c>
+      <c r="D41">
+        <v>118</v>
+      </c>
+      <c r="E41">
+        <v>138</v>
+      </c>
+      <c r="F41">
+        <v>133</v>
+      </c>
+      <c r="G41">
+        <v>136</v>
+      </c>
+      <c r="H41">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>6</v>
       </c>
-      <c r="B37">
+      <c r="B42">
+        <v>8</v>
+      </c>
+      <c r="C42">
+        <v>74</v>
+      </c>
+      <c r="D42">
+        <v>72</v>
+      </c>
+      <c r="E42">
+        <v>76</v>
+      </c>
+      <c r="F42">
+        <v>84</v>
+      </c>
+      <c r="G42">
+        <v>90</v>
+      </c>
+      <c r="H42">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>6</v>
+      </c>
+      <c r="B43">
+        <v>8</v>
+      </c>
+      <c r="C43">
+        <v>66</v>
+      </c>
+      <c r="D43">
+        <v>70</v>
+      </c>
+      <c r="E43">
+        <v>76</v>
+      </c>
+      <c r="F43">
+        <v>87</v>
+      </c>
+      <c r="G43">
+        <v>86</v>
+      </c>
+      <c r="H43">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>6</v>
+      </c>
+      <c r="B44">
+        <v>9</v>
+      </c>
+      <c r="C44">
+        <v>71</v>
+      </c>
+      <c r="D44">
+        <v>68</v>
+      </c>
+      <c r="E44">
+        <v>72</v>
+      </c>
+      <c r="F44">
+        <v>77</v>
+      </c>
+      <c r="G44">
+        <v>72</v>
+      </c>
+      <c r="H44">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>6</v>
+      </c>
+      <c r="B45">
+        <v>9</v>
+      </c>
+      <c r="C45">
+        <v>70</v>
+      </c>
+      <c r="D45">
+        <v>68</v>
+      </c>
+      <c r="E45">
+        <v>73</v>
+      </c>
+      <c r="F45">
+        <v>75</v>
+      </c>
+      <c r="G45">
+        <v>70</v>
+      </c>
+      <c r="H45">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>6</v>
+      </c>
+      <c r="B46">
+        <v>10</v>
+      </c>
+      <c r="C46">
+        <v>72</v>
+      </c>
+      <c r="D46">
+        <v>70</v>
+      </c>
+      <c r="E46">
+        <v>74</v>
+      </c>
+      <c r="F46">
+        <v>79</v>
+      </c>
+      <c r="G46">
+        <v>76</v>
+      </c>
+      <c r="H46">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>6</v>
+      </c>
+      <c r="B47">
+        <v>10</v>
+      </c>
+      <c r="C47">
+        <v>71</v>
+      </c>
+      <c r="D47">
+        <v>69</v>
+      </c>
+      <c r="E47">
+        <v>69</v>
+      </c>
+      <c r="F47">
+        <v>78</v>
+      </c>
+      <c r="G47">
+        <v>71</v>
+      </c>
+      <c r="H47">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>6</v>
+      </c>
+      <c r="B48">
         <v>11</v>
       </c>
-      <c r="C37">
+      <c r="C48">
+        <v>72</v>
+      </c>
+      <c r="D48">
+        <v>76</v>
+      </c>
+      <c r="E48">
+        <v>69</v>
+      </c>
+      <c r="F48">
+        <v>74</v>
+      </c>
+      <c r="G48">
+        <v>75</v>
+      </c>
+      <c r="H48">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>6</v>
+      </c>
+      <c r="B49">
+        <v>11</v>
+      </c>
+      <c r="C49">
         <v>70</v>
       </c>
-      <c r="D37">
+      <c r="D49">
         <v>77</v>
       </c>
-      <c r="E37">
+      <c r="E49">
         <v>70</v>
       </c>
-      <c r="F37">
+      <c r="F49">
         <v>74</v>
       </c>
-      <c r="G37">
+      <c r="G49">
         <v>73</v>
       </c>
-      <c r="H37">
+      <c r="H49">
         <v>79</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H37">
-    <sortCondition ref="A2:A37"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:H55">
+    <sortCondition ref="A5:A55"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8647,8 +9435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{872A1278-AF11-4598-BBDF-3C7E9575775C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>